<commit_message>
File format for resonance frequency finder
</commit_message>
<xml_diff>
--- a/eeg_recordings/vibro_tactile_27_12_2020/trial_02/repeated_k_fold_window_size.xlsx
+++ b/eeg_recordings/vibro_tactile_27_12_2020/trial_02/repeated_k_fold_window_size.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\EEG_GUI_OpenBCI\eeg_recordings\vibro_tactile_27_12_2020\trial_02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A1B0C5-BAC1-4C51-A512-A8EC157FACB7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA8095A-6E39-4AB8-A58A-CFB0E6833507}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>

<commit_message>
Resonance finder filter padding issue
</commit_message>
<xml_diff>
--- a/eeg_recordings/vibro_tactile_27_12_2020/trial_02/repeated_k_fold_window_size.xlsx
+++ b/eeg_recordings/vibro_tactile_27_12_2020/trial_02/repeated_k_fold_window_size.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\EEG_GUI_OpenBCI\eeg_recordings\vibro_tactile_27_12_2020\trial_02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA8095A-6E39-4AB8-A58A-CFB0E6833507}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED728333-414E-4DAF-A9AB-CF789A661564}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3180,7 +3180,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X23" sqref="X23"/>
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>